<commit_message>
reformat GO information files
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/proteinevoutk20@312 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/pkg/Result/GOTermFunction.xlsx
+++ b/pkg/Result/GOTermFunction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1440" windowWidth="24160" windowHeight="13340" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="13800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="GOTermFunction.xls" sheetId="1" r:id="rId1"/>
@@ -434,6 +434,10 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">

</xml_diff>